<commit_message>
takes reference stores and displays
</commit_message>
<xml_diff>
--- a/Teams/scripture memorise.xlsx
+++ b/Teams/scripture memorise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryannleslie/Documents/Study/cse210/Teams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704558DF-D3D0-8643-A05B-5B0CEE3718F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF675898-E8D8-C446-A31F-8607E994B182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="500" windowWidth="26920" windowHeight="16940" xr2:uid="{DA2A1C0E-80A9-384D-AC35-0DE456B9A203}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="26920" windowHeight="16940" xr2:uid="{DA2A1C0E-80A9-384D-AC35-0DE456B9A203}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>HideWords(): void</t>
   </si>
   <si>
-    <t>GetRenderedText() : string</t>
-  </si>
-  <si>
     <t>IsCompletelyHidden(): void</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>9. Ends on quit or all words hidden</t>
+  </si>
+  <si>
+    <t>GetRenderedText() : void</t>
   </si>
 </sst>
 </file>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23632299-6C99-E447-B094-BA362B6E2400}">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,37 +594,37 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
@@ -635,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>2</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3"/>
       <c r="E8" s="3" t="s">
@@ -666,73 +666,73 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>